<commit_message>
added new file for excel testing
</commit_message>
<xml_diff>
--- a/Selenium_ExcelDriven/data/demoData.xlsx
+++ b/Selenium_ExcelDriven/data/demoData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Testcases</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>bvnh</t>
-  </si>
-  <si>
-    <t>kjljk</t>
   </si>
   <si>
     <t>hjygu</t>
@@ -134,11 +131,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,7 +436,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -469,7 +469,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -483,7 +483,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -493,11 +493,11 @@
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
+      <c r="C4" s="4">
+        <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -508,10 +508,10 @@
         <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>